<commit_message>
Still working through the countries
</commit_message>
<xml_diff>
--- a/FoundData/BrazilDataInvestigation.xlsx
+++ b/FoundData/BrazilDataInvestigation.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Documents/GBAD/Data Quality Insights Project Folder/GBADsDataQualityInsights/FoundData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEF01F1-51F1-5F45-8265-05E42300618A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A439FD-AB2B-4343-9A3C-273940CF555A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{F9FC2081-E6B3-F148-9836-5A112ADB79DD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{F9FC2081-E6B3-F148-9836-5A112ADB79DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="84">
   <si>
     <t>Country</t>
   </si>
@@ -71,36 +71,18 @@
     <t>https://www.publish.csiro.au/an/AN14280</t>
   </si>
   <si>
-    <t>The paper Progress in the Brazilian cattle industry: an analysis of the Agricultural Censuses database identified that ther was 128 million cattle in Brazil in 1985, FAOSTAT said there was 124. This is less than a 2 percent difference which is really close.</t>
-  </si>
-  <si>
     <t>https://www.publish.csiro.au/an/AN14281</t>
   </si>
   <si>
-    <t xml:space="preserve">The paper Progress in the Brazilian cattle industry: an analysis of the Agricultural Censuses database identified that ther was 160 million cattle in Brazil in 2006, FAOSTAT said there was 205. This is a somewhat significant difference in population numbers. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Cattle </t>
   </si>
   <si>
     <t>FAOSTAT, WOAH</t>
   </si>
   <si>
-    <t>The paper Progress in the Brazilian cattle industry: an analysis of the Agricultural Censuses database identified that ther was 128 million cattle in Brazil in 1985, FAOSTAT said there was 124. This is less than a 2 percent difference which is really clos</t>
-  </si>
-  <si>
     <t>https://agenciadenoticias.ibge.gov.br/en/component/content/article/2013-agencia-de-noticias/releases/22661-2017-ppm-cattle-herd-prevails-in-central-west-mato-grosso-leads-states.html?Itemid=6769</t>
   </si>
   <si>
-    <t xml:space="preserve">The USDA estimates there is 244,144,000 cattle in Brazil in 2020. FAOSTAT/WOAH say there is approximatl7 215 million cattle alive at that time. This is a pretty large difference. Given that the USDA is only an esimate and FAOSTAT and WOAH get there's from counting, the FOASTAT and WOAH are more likely to be accurate. </t>
-  </si>
-  <si>
-    <t>The USDA said that in 2018 Brazil had 232 million cattle. They do not say if this number is an estimate or a count. So althought this number is ~20 million higher than FAOSTAT and WOAH. Given that it could be an estimate and it's the only external source to show this number, FAOSTAT and WOAH seem to be reliable sources for population numbers.</t>
-  </si>
-  <si>
-    <t>https://www.ers.usda.gov/amber-waves/2019/july/brazil-once-again-becomes-the-world-s-largest-beef-exporter/</t>
-  </si>
-  <si>
     <t>1962-1973</t>
   </si>
   <si>
@@ -110,12 +92,6 @@
     <t>1974-2020</t>
   </si>
   <si>
-    <t>The FAOSTAT flags for these numbers is almost all forcasted or Unofficial. This means there is an increase in the likely hood that these numbers are not exact.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The FAOSTAT flags for these numbers are all official. This means they all got them from a reputable source and have a high degree of confidence and likelyhood of being true. </t>
-  </si>
-  <si>
     <t>Chickens</t>
   </si>
   <si>
@@ -125,15 +101,9 @@
     <t>1971-2020</t>
   </si>
   <si>
-    <t>The FAOSTAT flags for these numbers are all forcasted. This means there is an increase in the likely hood that these numbers are not exact.</t>
-  </si>
-  <si>
     <t>https://apps.fas.usda.gov/newgainapi/api/Report/DownloadReportByFileName?fileName=Livestock%20and%20Products%20Annual_Brasilia_Brazil_08-15-2021.pdf</t>
   </si>
   <si>
-    <t>There is no info on brazilian chickens anywhere!!!!!</t>
-  </si>
-  <si>
     <t>Pigs</t>
   </si>
   <si>
@@ -152,7 +122,172 @@
     <t>FAOSTAT shows an almost 4 million sheep drop between these two years. There is no mention of this population drop in historical record so it is most likely not true</t>
   </si>
   <si>
-    <t>All external sources for livestock in the country just measure animal production via slaughter weight. There is no external sources for animal population numbers</t>
+    <t>https://sidra.ibge.gov.br/tabela/3939</t>
+  </si>
+  <si>
+    <t>1975-2020</t>
+  </si>
+  <si>
+    <t>Very close to the numbers reported by Brazilian Institute of Geography and Statistics (IBGE)</t>
+  </si>
+  <si>
+    <t>FAOSTAT/WOAH</t>
+  </si>
+  <si>
+    <t>FAOSTAT has the exact same  sheep numbers as Brazilian Institute of Geography and Statistics (IBGE) after 1974. This most likely means that FAOSTAT just reports IBGE's numbers.</t>
+  </si>
+  <si>
+    <t>FAOSTAT and the Brazilian Institute of Geography and Statistics (IBGE) have almost identical population numbers for cattle this year</t>
+  </si>
+  <si>
+    <t>FAOSTAT and Brazilian Institute of Geography and Statistics (IBGE) differ this year by almost 10 million cattle. IBGE says there is 102 million cattle vs FAOSTAT which says there is 92 million cattle. Most likely there wasn't a 10 million cattle increase that IBGE said and it's close to the 90 million mark.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAOSTAT and Brazilian Institute of Geography and Statistics (IBGE) differ this year by almost 10 million cattle. IBGE says there is 102 million cattle vs FAOSTAT which says there is 92 million cattle. Most likely there wasn't a 10 million cattle increase </t>
+  </si>
+  <si>
+    <t>FAOSTAT and Brazilian Institute of Geography and Statistics (IBGE) differ this year by almost 7 million cattle. This is a lot closer than in 1975 but is still not identical. FAOSTAT is more likely to be true given that the population would have grown by 15 million cattle in two years according to IBGE which is unlikely. FAOSTAT seems like a much more reasonable growth rate.</t>
+  </si>
+  <si>
+    <t>WOAH</t>
+  </si>
+  <si>
+    <t>FAOSTAT, WOAH, and IBGE have almost identical population numbers for this year.</t>
+  </si>
+  <si>
+    <t>1977 - 2018</t>
+  </si>
+  <si>
+    <t>FAOSTAT appears to be reporting IBGE data for the dates listed as they have the same data points between these two years.</t>
+  </si>
+  <si>
+    <t>FAOSTAT and the Brazilian Institute of Geography and Statistics (IBGE) have almost identical population numbers for pigs this year</t>
+  </si>
+  <si>
+    <t>1975-2019</t>
+  </si>
+  <si>
+    <t>FAOSTAT and IBGE have identical data for these years. It is most likely that FAOSTAT is just reporting IBGE data.</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Since FAOSTAT is reporting IBGE data and its data varies widely compare to WOAH, it is more likely that FAOSTAT has more correct data that WOAH.</t>
+  </si>
+  <si>
+    <t>FAOSTAT and the Brazilian Institute of Geography and Statistics (IBGE) have almost identical population numbers for chickens this year</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3940</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3941</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3942</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3943</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3944</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3945</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3946</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3947</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3948</t>
+  </si>
+  <si>
+    <t>https://sidra.ibge.gov.br/tabela/3949</t>
+  </si>
+  <si>
+    <t>The paper Progress in the Brazilian cattle industry: an analysis of the Agricultural Censuses database identified that there was 128 million cattle in Brazil in 1985, FAOSTAT said there was 124. This is less than a 2 percent difference which is really close.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The paper Progress in the Brazilian cattle industry: an analysis of the Agricultural Censuses database identified that there was 160 million cattle in Brazil in 2006, FAOSTAT said there was 205. This is a somewhat significant difference in population numbers. </t>
+  </si>
+  <si>
+    <t>The paper Progress in the Brazilian cattle industry: an analysis of the Agricultural Censuses database identified that there was 128 million cattle in Brazil in 1985, FAOSTAT said there was 124. This is less than a 2 percent difference which is really clos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The USDA estimates there is 244,144,000 cattle in Brazil in 2020. FAOSTAT/WOAH say there is approximatl7 215 million cattle alive at that time. This is a pretty large difference. Given that the USDA is only an estimate and FAOSTAT and WOAH get there's from counting, the FOASTAT and WOAH are more likely to be accurate. </t>
+  </si>
+  <si>
+    <t>The USDA said that in 2018 Brazil had 232 million cattle. They do not say if this number is an estimate or a count. So although this number is ~20 million higher than FAOSTAT and WOAH. Given that it could be an estimate and it's the only external source to show this number, FAOSTAT and WOAH seem to be reliable sources for population numbers.</t>
+  </si>
+  <si>
+    <t>https://www.ers.usda.gov/amber-waves/2019/July/Brazil-once-again-becomes-the-world-s-largest-beef-exporter/</t>
+  </si>
+  <si>
+    <t>The FAOSTAT flags for these numbers is almost all forecasted or Unofficial. This means there is an increase in the likely hood that these numbers are not exact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The FAOSTAT flags for these numbers are all official. This means they all got them from a reputable source and have a high degree of confidence and likelihood of being true. </t>
+  </si>
+  <si>
+    <t>The FAOSTAT flags for these numbers are all forecasted. This means there is an increase in the likely hood that these numbers are not exact.</t>
+  </si>
+  <si>
+    <t>WOAH and IBGE have similar a data but WOAH is slightly larger</t>
+  </si>
+  <si>
+    <t>2014-2017</t>
+  </si>
+  <si>
+    <t>https://www.theguardian.com/world/2015/jan/23/brazil-worst-drought-history</t>
+  </si>
+  <si>
+    <t>Brazil had one of it's worst recorded droughts between 2014 and 2017. It was so severe the country had rolling blackouts, and had to let crops wither to allocate water for essential services. Given this we should see an impact in livestock populations for this time. Brazil's cattle is almost entirly grass fed so they should be more resistant to this since they eat grass and not by product of crops grown in the country. FAOSTAT reports the population to have grown by 2.5% over this time period. So it's a little higher than expected but not an unreasonable growth given the situation at the time.</t>
+  </si>
+  <si>
+    <t>Brazil had one of it's worst recorded droughts between 2014 and 2017. It was so severe the country had rolling blackouts, and had to let crops wither to allocate water for essential services. Given this we should see an impact in livestock populations for this time. However we see Brazils sheep population grow from 17.6-18.6 million. Which is a 5.7 percent growth. This appears high,especially given the severity of the drought and how the cattle population grew by a smaller amount over the same time period and cattle are Brazils highest livestock export so it would be assumed that they would get priority as well.</t>
+  </si>
+  <si>
+    <t>Brazil had one of it's worst recorded droughts between 2014 and 2017. It was so severe the country had rolling blackouts, and had to let crops wither to allocate water for essential services. Given this we should see an impact in livestock populations for this time. However we see Brazils pig population grow from 17.6-18.6 million. Which is a 5.7 percent growth. This appears high,especially given the severity of the drought and how the cattle population grew by a smaller amount over the same time period and cattle are Brazils highest livestock export so it would be assumed that they would get priority as well.</t>
+  </si>
+  <si>
+    <t>Brazil had one of it's worst recorded droughts between 2014 and 2017. It was so severe the country had rolling blackouts, and had to let crops wither to allocate water for essential services. Given this we should see an impact in livestock populations for this time. However we see Brazils chicken population grow from 1.73-1.83 billion which is a 5.9 percent growth. This appears high,especially given the severity of the drought and how the cattle population grew by a smaller amount over the same time period and cattle are Brazils highest livestock export so it would be assumed that they would get priority as well.</t>
+  </si>
+  <si>
+    <t>2014-2020</t>
+  </si>
+  <si>
+    <t>https://www.ecb.europa.eu/pub/pdf/other/eb201601_focus01.en.pdf</t>
+  </si>
+  <si>
+    <t>In 2014 Brazil had an economic crisis that causes the country to have a shrinking GDP. This would cause people to have less disposable incoming for luxuries including more premium meats like beef so we would expect to see this affect the supply of cattle because the supply would increase as less people would be buying beef. Then the supply should decrease to stablize prices to the new demand. This is exactly what we see post 2014. The population of cattle keeps increasing. Then after two years it decreases and then stagnates through 2020</t>
+  </si>
+  <si>
+    <t>In 2014 Brazil had an economic crisis that causes the country to have a shrinking GDP. This would cause people to have less disposable incoming for luxuries including more premium meats like beef, instead consumers would gravitate towards cheaper protein such as chickens. Given this shift in consumer demand we would expect to see the chicken population increase to meet this demand. FAOSTAT does show increased supply over this time which would make sense given the hypothesis of Brazilian consumers consuming more chicken due to the 2014 recession.</t>
+  </si>
+  <si>
+    <t>In 2014 Brazil had an economic crisis that causes the country to have a shrinking GDP. This would cause people to have less disposable incoming for luxuries including more premium meats like beef, instead consumers would gravitate towards cheaper protein such as pork. Given this shift in consumer demand we would expect to see the pig population increase to meet this demand. FAOSTAT does show increased supply over this time which would make sense given the hypothesis of Brazilian consumers consuming more pigs due to the 2014 recession.</t>
+  </si>
+  <si>
+    <t>2019-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2019 Jair Bolsonaro was elected president of Brazil. Among many other policies he championed, one significant one was reducing protections of indiginous groups and protections of the Amazon rainforest. These protections were a driving force in saving the Amazon from being burned to create grazing land for cattle. Given the increase of destruction and increase in grazing land for cattle, we would expect to see an increase in cattle population after he is elected, specifically  a year after since it takes time to burn a forest and let it regenerate into pasture for cattle. FAOSTAT shows a jump of 3 million cattle in 2020. This is a small difference of less than 1.5 percent. This does back the political climate at the time, the effects might be seen in a larger amount in future years. </t>
+  </si>
+  <si>
+    <t>2003-2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2003 Luiz Inácio Lula da Silva was elected as president of Brazil. One of the policies enacted by Lula was increasing protects for the Amazon Rainforest. Since one of the main reasons the Amazon Rainforest was ranchers would burn the forest to create pasture for their animals. So with Lula getting elected and increasing protection we should see a stagnation of the cattle population size. Looking at FAOSTAT's data we can see that the population of cattle fell post 2005, and slowly increased every year until 2010. So this would make sense given the political climate at this time. </t>
+  </si>
+  <si>
+    <t>https://www.cfr.org/in-brief/deforestation-brazils-amazon-has-reached-record-high-whats-being-done</t>
+  </si>
+  <si>
+    <t>https://successfulsocieties.princeton.edu/publications/credible-commitment-reducing-deforestation-brazilian-amazon-2003–2012</t>
   </si>
 </sst>
 </file>
@@ -511,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C075BE-C5A1-774B-BF2F-EDCBAD28FD4E}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="159" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -582,10 +717,10 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -593,22 +728,22 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>2017</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -622,16 +757,16 @@
         <v>2020</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -645,16 +780,16 @@
         <v>2018</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -665,7 +800,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -674,10 +809,10 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -685,10 +820,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -697,10 +832,10 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -708,10 +843,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -720,7 +855,10 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>65</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -728,10 +866,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -740,7 +878,10 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -748,10 +889,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -760,10 +901,10 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -771,10 +912,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -783,20 +924,562 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>1974</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1975</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>1975</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>1976</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>2020</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>2019</v>
+      </c>
+      <c r="D20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
         <v>38</v>
+      </c>
+      <c r="G20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>2018</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>2020</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>2020</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>